<commit_message>
begin gemaakt aan eigen website
</commit_message>
<xml_diff>
--- a/laravel_user_stories_v20191120.xlsx
+++ b/laravel_user_stories_v20191120.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP\htdocs\bap\periode2.1\bap-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8478C4-8C92-419D-AA93-8BAE8B9064C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245EA832-1A47-4669-BFD4-0F33812378A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{96E4F204-A96B-B442-B776-0E7F469FE00D}"/>
   </bookViews>
@@ -1715,7 +1715,7 @@
     </row>
     <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>21</v>
@@ -3082,6 +3082,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8D01017B67FFC40B6EAF835C0079E48" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c7194cc31030e2712d76c2006e0d75af">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="584c6f05-645a-45c2-af5b-a2298cf6e1b5" xmlns:ns3="5c2aeaab-3434-48d9-b2ba-99c708216bcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="420f24c0cdcfc5bd7329cba19e0bdf1c" ns2:_="" ns3:_="">
     <xsd:import namespace="584c6f05-645a-45c2-af5b-a2298cf6e1b5"/>
@@ -3284,22 +3299,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C4C429B-C437-4A37-B7CA-137886FFB6B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="5c2aeaab-3434-48d9-b2ba-99c708216bcd"/>
+    <ds:schemaRef ds:uri="584c6f05-645a-45c2-af5b-a2298cf6e1b5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2490BF6-BAD1-45FA-8E2E-1DC0E56639F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C62A3BA8-675C-43E7-9E30-618B42A3DB6A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3316,29 +3341,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2490BF6-BAD1-45FA-8E2E-1DC0E56639F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C4C429B-C437-4A37-B7CA-137886FFB6B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="5c2aeaab-3434-48d9-b2ba-99c708216bcd"/>
-    <ds:schemaRef ds:uri="584c6f05-645a-45c2-af5b-a2298cf6e1b5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
blok 10 userstories van de website af
</commit_message>
<xml_diff>
--- a/laravel_user_stories_v20191120.xlsx
+++ b/laravel_user_stories_v20191120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP\htdocs\bap\periode2.1\bap-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245EA832-1A47-4669-BFD4-0F33812378A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD245A12-CBF2-4828-A933-54CC3C4C141E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{96E4F204-A96B-B442-B776-0E7F469FE00D}"/>
   </bookViews>
@@ -1533,8 +1533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F8C07C-95E6-5F45-AA16-00A7B9F9E844}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="94" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="94" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>27</v>
@@ -1876,7 +1876,7 @@
     </row>
     <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>28</v>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>29</v>
@@ -1922,7 +1922,7 @@
     </row>
     <row r="17" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>30</v>
@@ -1945,7 +1945,7 @@
     </row>
     <row r="18" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
opdracht af zover ik het kon maken
</commit_message>
<xml_diff>
--- a/laravel_user_stories_v20191120.xlsx
+++ b/laravel_user_stories_v20191120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP\htdocs\bap\periode2.1\bap-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD245A12-CBF2-4828-A933-54CC3C4C141E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD62C24-F863-4A0B-8CC9-BB5EA7ED665B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{96E4F204-A96B-B442-B776-0E7F469FE00D}"/>
   </bookViews>
@@ -408,9 +408,6 @@
     <t>zodat ik controle heb over de inhoud</t>
   </si>
   <si>
-    <t>bij een item in et CMS kunnen aangeven of die zichtbaar of niet zichtbaar is</t>
-  </si>
-  <si>
     <t>Blok</t>
   </si>
   <si>
@@ -598,6 +595,9 @@
   </si>
   <si>
     <t>Routing &amp; Views</t>
+  </si>
+  <si>
+    <t>bij een item in het CMS kunnen aangeven of die zichtbaar of niet zichtbaar is</t>
   </si>
 </sst>
 </file>
@@ -1533,8 +1533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F8C07C-95E6-5F45-AA16-00A7B9F9E844}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="94" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="94" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1557,7 +1557,7 @@
         <v>35</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
@@ -1770,7 +1770,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>27</v>
@@ -1862,16 +1862,16 @@
         <v>10</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.4">
@@ -1948,7 +1948,7 @@
         <v>39</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18" s="6">
         <v>10</v>
@@ -1968,7 +1968,7 @@
     </row>
     <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>31</v>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="20" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>32</v>
@@ -2006,15 +2006,15 @@
         <v>11</v>
       </c>
       <c r="F20" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>33</v>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>56</v>
@@ -2060,7 +2060,7 @@
     </row>
     <row r="23" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>62</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="24" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>63</v>
@@ -2098,15 +2098,15 @@
         <v>11</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>80</v>
@@ -2129,7 +2129,7 @@
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>81</v>
@@ -2152,7 +2152,7 @@
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>82</v>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>85</v>
@@ -2247,7 +2247,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C31" s="6">
         <v>12</v>
@@ -2271,7 +2271,7 @@
         <v>37</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C32" s="6">
         <v>12</v>
@@ -2295,7 +2295,7 @@
         <v>37</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C33" s="6">
         <v>13</v>
@@ -2307,10 +2307,10 @@
         <v>9</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H33" s="9"/>
     </row>
@@ -2319,7 +2319,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C34" s="6">
         <v>13</v>
@@ -2342,7 +2342,7 @@
         <v>37</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C35" s="6">
         <v>14</v>
@@ -2365,7 +2365,7 @@
         <v>37</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C36" s="6">
         <v>14</v>
@@ -2377,10 +2377,10 @@
         <v>9</v>
       </c>
       <c r="F36" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="21" x14ac:dyDescent="0.4">
@@ -2396,7 +2396,7 @@
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G38" s="2"/>
     </row>
@@ -2606,7 +2606,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2646,10 +2646,10 @@
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>68</v>
@@ -2658,10 +2658,10 @@
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.4">
@@ -2669,7 +2669,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>67</v>
@@ -2689,7 +2689,7 @@
         <v>37</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>93</v>
@@ -2698,7 +2698,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>124</v>
+        <v>187</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>112</v>
@@ -2709,7 +2709,7 @@
         <v>37</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>52</v>
@@ -2721,7 +2721,7 @@
         <v>92</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.4">
@@ -2729,19 +2729,19 @@
         <v>37</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.4">
@@ -2749,7 +2749,7 @@
         <v>37</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>67</v>
@@ -2758,10 +2758,10 @@
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.4">
@@ -2769,7 +2769,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>52</v>
@@ -2778,10 +2778,10 @@
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.4">
@@ -2789,19 +2789,19 @@
         <v>37</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.4">
@@ -2809,19 +2809,19 @@
         <v>37</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.4">
@@ -2829,39 +2829,39 @@
         <v>37</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.4">
@@ -2869,19 +2869,19 @@
         <v>37</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.4">
@@ -2889,19 +2889,19 @@
         <v>37</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.4">
@@ -2923,7 +2923,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -3082,21 +3082,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8D01017B67FFC40B6EAF835C0079E48" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c7194cc31030e2712d76c2006e0d75af">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="584c6f05-645a-45c2-af5b-a2298cf6e1b5" xmlns:ns3="5c2aeaab-3434-48d9-b2ba-99c708216bcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="420f24c0cdcfc5bd7329cba19e0bdf1c" ns2:_="" ns3:_="">
     <xsd:import namespace="584c6f05-645a-45c2-af5b-a2298cf6e1b5"/>
@@ -3299,32 +3284,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C4C429B-C437-4A37-B7CA-137886FFB6B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="5c2aeaab-3434-48d9-b2ba-99c708216bcd"/>
-    <ds:schemaRef ds:uri="584c6f05-645a-45c2-af5b-a2298cf6e1b5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2490BF6-BAD1-45FA-8E2E-1DC0E56639F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C62A3BA8-675C-43E7-9E30-618B42A3DB6A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3341,4 +3316,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2490BF6-BAD1-45FA-8E2E-1DC0E56639F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C4C429B-C437-4A37-B7CA-137886FFB6B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="5c2aeaab-3434-48d9-b2ba-99c708216bcd"/>
+    <ds:schemaRef ds:uri="584c6f05-645a-45c2-af5b-a2298cf6e1b5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>